<commit_message>
Excel files read as records and translation now tracks attempts
</commit_message>
<xml_diff>
--- a/excel-data-files/currrency-translate-gl-account-balances.xlsx
+++ b/excel-data-files/currrency-translate-gl-account-balances.xlsx
@@ -1,91 +1,93 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardguy/r/oracleplaywright/excel-data-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lchaplin\Code\oracleplaywright\excel-data-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F858FC-79BB-E34A-9825-96F780CC57AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083D1820-6381-40B6-8917-693D03E57A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="2180" windowWidth="29060" windowHeight="17100" activeTab="2" xr2:uid="{39C55B49-5ADB-CF4F-8459-6E15E59B12DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="3" r:id="rId1"/>
-    <sheet name="Setup" sheetId="1" r:id="rId2"/>
-    <sheet name="Loop" sheetId="2" r:id="rId3"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId1"/>
+    <sheet name="Setup" sheetId="2" r:id="rId2"/>
+    <sheet name="Loop" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+  <si>
+    <t>Instructions:</t>
+  </si>
+  <si>
+    <t>This data file must have the same filename as the Playwright test script, and must be stored in the excel-data-files folder.</t>
+  </si>
+  <si>
+    <t>Use the Setup sheet (Column B) for the values required only once. (Titles in column A can be whatever you like).</t>
+  </si>
+  <si>
+    <t>Use the Loop sheet (Rows 2 onwards) for values required many times. (Titles on Row 1 can be whatever you like).</t>
+  </si>
+  <si>
+    <t>Any other format will not work!</t>
+  </si>
   <si>
     <t>url</t>
   </si>
   <si>
+    <t>https://iahdme-test.fa.ocs.oraclecloud.com/fscmUI/faces/FuseOverview</t>
+  </si>
+  <si>
     <t>newProcessName</t>
   </si>
   <si>
+    <t>translate general Ledger account balances</t>
+  </si>
+  <si>
     <t>dataAccessSet</t>
   </si>
   <si>
+    <t>HK ACTUALS HKD Apr</t>
+  </si>
+  <si>
     <t>ledgerOrLedgerSet</t>
   </si>
   <si>
     <t>targetCurrency</t>
   </si>
   <si>
+    <t>GBP Pound Sterling</t>
+  </si>
+  <si>
+    <t>Test Attempt Count</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
     <t>accountingPeriods</t>
   </si>
   <si>
     <t>balancingSegment</t>
   </si>
   <si>
-    <t>translate general Ledger account balances</t>
-  </si>
-  <si>
-    <t>Use the Loop sheet (Rows 2 onwards) for values required many times. (Titles on Row 1 can be whatever you like).</t>
-  </si>
-  <si>
-    <t>Instructions:</t>
-  </si>
-  <si>
-    <t>Use the Setup sheet (Column B) for the values required only once. (Titles in column A can be whatever you like).</t>
-  </si>
-  <si>
-    <t>Any other format will not work!</t>
-  </si>
-  <si>
-    <t>This data file must have the same filename as the Playwright test script, and must be stored in the excel-data-files folder.</t>
-  </si>
-  <si>
-    <t>https://iahdme-test.fa.ocs.oraclecloud.com/fscmUI/faces/FuseOverview</t>
-  </si>
-  <si>
-    <t>GBP Pound Sterling</t>
-  </si>
-  <si>
-    <t>HK ACTUALS HKD Apr</t>
+    <t>REQUESTID</t>
+  </si>
+  <si>
+    <t>STARTTIME</t>
+  </si>
+  <si>
+    <t>ENDTIME</t>
+  </si>
+  <si>
+    <t>RESULT</t>
   </si>
   <si>
     <t>Apr-18</t>
@@ -101,7 +103,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,41 +111,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -155,24 +129,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -500,175 +467,188 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD33EC5-03CB-D544-9EAA-46900CFD2381}">
-  <dimension ref="A1:B27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:B27" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5.83203125" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="3"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4" t="s">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:B5 A6" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B25D91-67B5-EF48-9DB9-A33972D99E99}">
-  <dimension ref="A1:B5"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>270000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>270000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>270000</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{14A53803-7D5F-FF41-AFDE-9D9DB84BDB7A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:G1 A3:G4 A2:F2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA25780A-EA5B-9148-8FFA-6154678F87EB}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2">
-        <v>270000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3">
-        <v>270000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4">
-        <v>270000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{ea60d57e-af5b-4752-ac57-3e4f28ca11dc}" enabled="1" method="Standard" siteId="{36da45f1-dd2c-4d1f-af13-5abe46b99921}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>